<commit_message>
Update to Code and Error tracker
</commit_message>
<xml_diff>
--- a/General/Usask Conversion Code/Code Error Tracker.xlsx
+++ b/General/Usask Conversion Code/Code Error Tracker.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\OER-mechanics-webwork\General\Usask Conversion Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FF6196-9F8A-41CE-B680-E86A4E14A3AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A63826-823E-41B4-8D60-C4B6BCFF4451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CDAD8834-48C0-48D7-835D-DC8026F9B951}"/>
+    <workbookView xWindow="9144" yWindow="768" windowWidth="13860" windowHeight="8964" xr2:uid="{CDAD8834-48C0-48D7-835D-DC8026F9B951}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="problem3" localSheetId="0">Sheet1!$B$20</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
   <si>
     <t>Filename</t>
   </si>
@@ -104,7 +107,311 @@
     <t>Equation formatting issue</t>
   </si>
   <si>
-    <t>in progress</t>
+    <t>/STATICS-ASV010101faefa0460d484e039accabc59f8495a0.pg</t>
+  </si>
+  <si>
+    <t>Images not showing</t>
+  </si>
+  <si>
+    <t>STATICS-ASV0102013147e0a182474ffdab67f6e436d9b4.pg</t>
+  </si>
+  <si>
+    <t>Note: If problems have a similar error, one problem would be used to fix the error.</t>
+  </si>
+  <si>
+    <t>STATICS-ASV020101cfaee54099bd478f9ee7bfe6c5e80e9c.pg</t>
+  </si>
+  <si>
+    <t>syntax error at (eval 2347) line 47, near ""\\($\\)()"\"
+Missing right curly or square bracket at (eval 2347) line 73, at end of line</t>
+  </si>
+  <si>
+    <t>STATICS-ASV030103a50cd3cb0dfd4eaa8a0f7ce13f18c8e.pg</t>
+  </si>
+  <si>
+    <t>Image missing</t>
+  </si>
+  <si>
+    <t>General Issues</t>
+  </si>
+  <si>
+    <t>Photo Resizing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATICS-ASV0601037e74a478d8b84ae9b4c029df53e6bb40.png </t>
+  </si>
+  <si>
+    <t>STATICS-ASV070102f2106e060e1144ae914b067fdcc478a8.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> syntax error at (eval 2347) line 54, at EOF
+syntax error at (eval 2347) line 62, at EOF</t>
+  </si>
+  <si>
+    <t>STATICS-ASV07020210d594f202ca4507a9979a612e053ea4.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> syntax error at (eval 4940) line 54, at EOF
+syntax error at (eval 4940) line 62, at EOF</t>
+  </si>
+  <si>
+    <t>$ans1=[B]\right;</t>
+  </si>
+  <si>
+    <t>/STATICS-ASV070501c07ef6124129489ba07933e653780c19.pg</t>
+  </si>
+  <si>
+    <t>STATICS-ASV0801011be4e32fa6a94bd5865a72f2119388e.pg</t>
+  </si>
+  <si>
+    <t>Can't locate object method "qquad" via package "C_y" (perhaps you forgot to load "C_y"?) at line 47 of (eval 2347)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATICS-CVF0302043bb5d566bd604f4cacbded22c22c5710.png </t>
+  </si>
+  <si>
+    <t>STATICS-CVF0307025ead0a4ae7ac42a7a161dddb43697440.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> syntax error at (eval 2761) line 57, near "}{"</t>
+  </si>
+  <si>
+    <t>STATICS-CVF050102caf6faa9514846b69b0c9765fdffb5b8.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compilation errorsyntax error at (eval 3337) line 62, near "gamma\"</t>
+  </si>
+  <si>
+    <t>STATICS-CVF0601010197111142264b80bf14923f37093e36.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> syntax error at (eval 2347) line 57, near "$Acos("</t>
+  </si>
+  <si>
+    <t>STATICS-CVF0701011fe44fc2c52044b5897c1013f4837d2c.pg</t>
+  </si>
+  <si>
+    <t>STATICS-PSE01030104c270248a2c4db5a015d89af6f12600.png missing resource path</t>
+  </si>
+  <si>
+    <t>missing resource path</t>
+  </si>
+  <si>
+    <t>STATICS-PSE030101063c9edeaa694b52a0aa59d3a1fe24b2.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> \overrightarrow{\(F_1}\)</t>
+  </si>
+  <si>
+    <t>F2−→ =(-3\)i^+0j^)N</t>
+  </si>
+  <si>
+    <t>STATICS-PSE0301046aac19163087406093cb95c118c78ac4.pg</t>
+  </si>
+  <si>
+    <t>STATICS-PSE0501029328bfc7cc3345e2b29c47578d8a787e.pg</t>
+  </si>
+  <si>
+    <t>failed to read file</t>
+  </si>
+  <si>
+    <t>STATICS-PSE050103a3d6475d12ff44b8b822803b2d2f0c43.pg</t>
+  </si>
+  <si>
+    <t>STATICS-PSE050201895116ae8d794581907f45b3d0c3aab4.pg</t>
+  </si>
+  <si>
+    <t>Answers not complete</t>
+  </si>
+  <si>
+    <t>STATICS-PSE0601018199ec40c7594421a499a63a7d453229.pg</t>
+  </si>
+  <si>
+    <t>STATICS-PSE060201210155d7d85445bcbd30dbcc9d4a138b.pg</t>
+  </si>
+  <si>
+    <t>Answer not determined</t>
+  </si>
+  <si>
+    <t>STATICS-PSE070402078e852225df4f0b9a6eb651fb8c133.pg</t>
+  </si>
+  <si>
+    <t>STATICS-PSE090101694d6380095442d98d4b3b7fd3526ec1.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F1=100\;\N (Formatting errors)</t>
+  </si>
+  <si>
+    <t>STATICS-PSE09010299a25a5d5684432ea2c00871a65bfa86.pg</t>
+  </si>
+  <si>
+    <t>Formatting Issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> k_{AC}=20\;\</t>
+  </si>
+  <si>
+    <t>STATICS-PSE0901038b6f3c25aa6a4c6a832c90acd12d4b7.pg</t>
+  </si>
+  <si>
+    <t>\;\mathrm{lb}</t>
+  </si>
+  <si>
+    <t>STATICS-PSE090202111f677f38664f6c935195bee8926b54.pg</t>
+  </si>
+  <si>
+    <t>STATICS-PSE090203ac2d299d85494232832160dafbf96d23.pg</t>
+  </si>
+  <si>
+    <t>STATICS-PSE090204508e02ce27cb46618714148b0d9301b6.pg</t>
+  </si>
+  <si>
+    <t>Consider the following scenario: --- The hook depicted in the image below has two ropes pulling on it. The first rope is pulling with a force F1=100\;\N and the second rope is pulling with a force F2=150\;\N. The angles \theta1 and \theta2 are 15\degreeand 10\degreerespectively. What is the magnitude of the resultant force acting on the hook due to the two ropes?</t>
+  </si>
+  <si>
+    <t>STATICS-PSE0903018633ffcdb2724b97b8db483b73ffba9e.pg</t>
+  </si>
+  <si>
+    <t>STATICS-PSE090302611a0c335b5c4158909cfbccf91184f6.pg</t>
+  </si>
+  <si>
+    <t>Inconsistency in answers</t>
+  </si>
+  <si>
+    <t>STATICS-PSE090304a1b1d667c0774368b2086ce7b74ef513.pg</t>
+  </si>
+  <si>
+    <t>∑{F}_y=0</t>
+  </si>
+  <si>
+    <t>STATICS-PSE1102024fa0fce603d2488e803bcfadd8c03729.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+a) ∑F⃗ x+\overrightarrow{F}_y+\overrightarrow{F}_z=0</t>
+  </si>
+  <si>
+    <t>STATICS-PSE1201011ddfa74e8c414b6dafe36e8888051d73.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ∑F⃗ xi^+F_yj^=0</t>
+  </si>
+  <si>
+    <t>∑{F}y=0</t>
+  </si>
+  <si>
+    <t>STATICS-PSE110301d2812919dff948d4b7c290f9374eaeb2.pg</t>
+  </si>
+  <si>
+    <t>STATICS-PSE11030279ee47716b8a40bb937e15d9998d5f59.pg</t>
+  </si>
+  <si>
+    <t>STATICS-PSE1303017b0251426b374232bb9aab25d682c056.pg</t>
+  </si>
+  <si>
+    <t>Numerical instead of MC</t>
+  </si>
+  <si>
+    <t>Fx , F_y, and f_z</t>
+  </si>
+  <si>
+    <t>STATICS-PSE1303026dab5d8b37c04f86b4ca6235c5d2b827.pg</t>
+  </si>
+  <si>
+    <t>STATICS-VDP010101854a6b3b21a7424f92cbfe466c0a4716.pg</t>
+  </si>
+  <si>
+    <t>\sqrt{(Ax)^2+(Ay)^2}+\sqrt{(Bx)^2+(By)^2}</t>
+  </si>
+  <si>
+    <t>cos^{-1}(\frac{C}{AB})</t>
+  </si>
+  <si>
+    <t>STATICS-VDP010201f5781e3e8c434ef2932d8462843af4ca.pg</t>
+  </si>
+  <si>
+    <t>cos^{-1}(\frac{Ax⋅ Bx+Ay⋅ By}{\sqrt{(Ax)^2+(Ay)^2}×\sqrt{(Bx)^2+(By)^2}})</t>
+  </si>
+  <si>
+    <t>STATICS-VDP01020229dee47004bb4a9686884a34957434fb.pg</t>
+  </si>
+  <si>
+    <t>STATICS-VDP0104018341ddba2dc241bea823420d793c4d94.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compilation errorsyntax error at (eval 4057) line 49, near ""d.  \\($A\\)\\(\\cos\\)(90^\\circ-\\($B\\)^\\circ)"\"
+Missing right curly or square bracket at (eval 4057) line 78, at end of line</t>
+  </si>
+  <si>
+    <t>STATICS-VDP0105012186a0315ccb4a2f807fd83267ff6a12.pg</t>
+  </si>
+  <si>
+    <t>\sqrt{(Bx)^2+(By)^2+(Bz)^2}</t>
+  </si>
+  <si>
+    <t>STATICS-VDP020101ab133da470db4cbea32c0265e77742ee.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> \text{sin}^{-1}(\frac{C}{AB})</t>
+  </si>
+  <si>
+    <t>STATICS-VDP0202013c3709610c3042caa103c0ad91c90997.pg</t>
+  </si>
+  <si>
+    <t>"a. Good job. The dot product of two vectors would be positive if the angle between them is acute (\(\theta\)&lt;90^\circ). The solution to this question is provided below. ");</t>
+  </si>
+  <si>
+    <t>STATICS-VDP030101c40b64e5836e4695b1121664f326d2f9.pg</t>
+  </si>
+  <si>
+    <t>STATICS-VDP040106c353e3c4de8b4ddcb07af48055d1ddaa.pg</t>
+  </si>
+  <si>
+    <t>STATICS-VDP040203a7931ccaf7414321bb05e80b0c679e80.png</t>
+  </si>
+  <si>
+    <t>Image is missing</t>
+  </si>
+  <si>
+    <t>Errors parsing PGML:
+'_' was not closed before paragraph ends
+'_' was not closed before paragraph ends
+Error parsing answer: 'HASH' is not defined in this context; see position 1 of formula</t>
+  </si>
+  <si>
+    <t>STATICS-VDP05030188ba9273a86c405484a844de6fbe5975.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compilation errorsyntax error at (eval 2347) line 62, near "cdot\"
+syntax error at (eval 2347) line 62, near "}}"</t>
+  </si>
+  <si>
+    <t>STATICS-VDP0701010e4b62fd7050410fa0a648431ce6ae0.pg</t>
+  </si>
+  <si>
+    <t>__
+ ^circ</t>
+  </si>
+  <si>
+    <t>STATICS-VDP0XXX25e0839c2b60471da8b16384f2c17953.pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A⃗ =(hat{−7i}+−5j^+−8k^) and B⃗ =(hat{−5i}+6j^+−4k^). </t>
+  </si>
+  <si>
+    <t>STATICS-VDP0XXXa4c1ff1276b74bd884541e61d20d3e43.pg</t>
+  </si>
+  <si>
+    <t>Untitled7bc9668bed5142c9a7b76ec7700c8165.pg</t>
+  </si>
+  <si>
+    <t>File cannot be found</t>
+  </si>
+  <si>
+    <t>decode circle into utf-8</t>
+  </si>
+  <si>
+    <t>fixed</t>
   </si>
 </sst>
 </file>
@@ -481,10 +788,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BB84F7-F3C2-4244-AFCB-4F866F2C7CEE}">
-  <dimension ref="A1:C11"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,7 +800,7 @@
     <col min="1" max="16384" width="28.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -502,8 +810,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -511,10 +822,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -525,7 +842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -536,7 +853,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -547,7 +864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -558,7 +875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -569,7 +886,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -580,7 +897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -591,7 +908,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -602,12 +919,522 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>